<commit_message>
AURELION VERSIÓN 2: Incorporación de módulo para reportes gerenciales, tabla maestra para analizar todo el dataset.
</commit_message>
<xml_diff>
--- a/Edwar Jaramillo - Aurelion/database/db_limpia/clientes_actualizado.xlsx
+++ b/Edwar Jaramillo - Aurelion/database/db_limpia/clientes_actualizado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2764,6 +2764,25 @@
         <v>45026</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Edwar</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>edwar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>